<commit_message>
Added cross-ref to first half of year
</commit_message>
<xml_diff>
--- a/katamarous source/months.xlsx
+++ b/katamarous source/months.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brett/Documents/psalmody/katamarous source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bslote\Documents\psalmody\katamarous source\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="7540" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="1020" yWindow="7536" windowWidth="28800" windowHeight="17604" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>September</t>
   </si>
@@ -138,13 +138,52 @@
   </si>
   <si>
     <t>Ⲕⲟⲩϫⲓ ⲛ̀ⲁ̀ⲃⲟⲧ</t>
+  </si>
+  <si>
+    <t>Tut</t>
+  </si>
+  <si>
+    <t>Babah</t>
+  </si>
+  <si>
+    <t>Hatur</t>
+  </si>
+  <si>
+    <t>Kiahk</t>
+  </si>
+  <si>
+    <t>Tubah</t>
+  </si>
+  <si>
+    <t>Amshir</t>
+  </si>
+  <si>
+    <t>Baramhat</t>
+  </si>
+  <si>
+    <t>Baramouda</t>
+  </si>
+  <si>
+    <t>Bashons</t>
+  </si>
+  <si>
+    <t>Baunah</t>
+  </si>
+  <si>
+    <t>Abib</t>
+  </si>
+  <si>
+    <t>Mesra</t>
+  </si>
+  <si>
+    <t>Nasi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -196,6 +235,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -464,15 +506,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D15"/>
+  <dimension ref="B3:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="3" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:5">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -482,8 +524,11 @@
       <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="24">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -493,8 +538,11 @@
       <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="24">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -504,8 +552,11 @@
       <c r="D5" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="24">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -515,8 +566,11 @@
       <c r="D6" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="24">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -526,8 +580,11 @@
       <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="24">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -537,8 +594,11 @@
       <c r="D8" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="24">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -548,8 +608,11 @@
       <c r="D9" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="24">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -559,8 +622,11 @@
       <c r="D10" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="24">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -570,8 +636,11 @@
       <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="24">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -581,8 +650,11 @@
       <c r="D12" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="24">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -592,8 +664,11 @@
       <c r="D13" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" ht="24">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -603,16 +678,23 @@
       <c r="D14" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="24" x14ac:dyDescent="0.5">
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="24">
       <c r="C15" t="s">
         <v>24</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>